<commit_message>
first test version and add delete rows task
</commit_message>
<xml_diff>
--- a/app/assets/xlsx/clients.xlsx
+++ b/app/assets/xlsx/clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId4"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Tél 2</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
   <si>
     <t>Notes</t>
@@ -46,19 +49,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="3">
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
-      <color theme="1"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -79,21 +82,21 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="false" shrinkToFit="false" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -165,53 +168,53 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
-                <a:satMod val="105000"/>
-                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
-                <a:satMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
+                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
-                <a:satMod val="109000"/>
-                <a:lumMod val="105000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
-                <a:satMod val="120000"/>
-                <a:lumMod val="99000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -246,7 +249,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -269,16 +272,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
-                <a:satMod val="150000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
-                <a:satMod val="130000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -289,7 +292,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -300,18 +303,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="false" summaryRight="false"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col customWidth="1" min="6" max="6" width="14.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="false">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -336,70 +338,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" customFormat="false">
-      <c r="A2" s="0" t="str">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="str">
-        <v>19/06/2024</v>
-      </c>
-      <c r="C2" s="0" t="str">
-        <v>Timothée</v>
-      </c>
-      <c r="D2" s="0" t="str">
-        <v>Régis</v>
-      </c>
-      <c r="E2" s="0" t="str">
-        <v>registimothee@gmail.com</v>
-      </c>
-      <c r="F2" s="0" t="str">
-        <v>01/09/1993</v>
-      </c>
-      <c r="G2" s="0" t="str">
-        <v>0769181771</v>
-      </c>
-      <c r="H2" s="0" t="str">
-        <v>0145065828</v>
-      </c>
-      <c r="I2" s="0" t="str">
-        <v>Réinscritption</v>
-      </c>
-      <c r="J2" s="0" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:10" customFormat="false">
-      <c r="A4" s="0" t="str">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="str">
-        <v>19/06/2024</v>
-      </c>
-      <c r="C4" s="0" t="str">
-        <v>Alexis</v>
-      </c>
-      <c r="D4" s="0" t="str">
-        <v>Régis</v>
-      </c>
-      <c r="E4" s="0" t="str">
-        <v>alexis.regis@hotmail.fr</v>
-      </c>
-      <c r="F4" s="0" t="str">
-        <v>21/11/1997</v>
-      </c>
-      <c r="G4" s="0" t="str">
-        <v>0607447714</v>
-      </c>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0" t="str">
-        <v/>
-      </c>
-      <c r="J4" s="0" t="str">
-        <v/>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add target blank to submit
</commit_message>
<xml_diff>
--- a/app/assets/xlsx/clients.xlsx
+++ b/app/assets/xlsx/clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <si>
     <t>ID</t>
   </si>
@@ -49,19 +49,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -82,21 +82,21 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="false" shrinkToFit="false" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -168,53 +168,53 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="67000"/>
+                <a:satMod val="105000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="73000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="81000"/>
+                <a:satMod val="109000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="78000"/>
+                <a:satMod val="120000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -249,7 +249,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -272,16 +272,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:shade val="98000"/>
                 <a:satMod val="150000"/>
-                <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:shade val="90000"/>
                 <a:satMod val="130000"/>
-                <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -292,7 +292,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -303,17 +303,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="false" summaryRight="false"/>
   </sheetPr>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="14.75"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" customFormat="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -343,6 +344,38 @@
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" customFormat="false">
+      <c r="A2" s="0" t="str">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <v>21/08/2024</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <v>Timothée</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <v>Régis</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <v>registimothee@gmail.com</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <v>08/08/1990</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <v>0769181771</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <v/>
+      </c>
+      <c r="I2" s="0" t="str">
+        <v>Nouveau client</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>